<commit_message>
Tipo de servicio: "Diseño o modelado"
Actualización del cotizador con el campo para subir imagenes en Diseño o modelado y separación de tipos de servicio.
</commit_message>
<xml_diff>
--- a/resources/Template Capacitacion.xlsx
+++ b/resources/Template Capacitacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capti\Documents\GitHub\projectManagemt\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09507183-B15B-40A2-BF10-D9E0C597B1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B8B7E0-8D3D-4EF1-9DCA-8A4568167C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quota" sheetId="1" r:id="rId1"/>
@@ -171,7 +171,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +324,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Lato"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -540,7 +546,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -635,6 +640,24 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -644,10 +667,6 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -662,20 +681,7 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1417,7 +1423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -1438,10 +1444,10 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="33"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:7" ht="34.5" customHeight="1">
       <c r="A2" s="1"/>
@@ -1449,96 +1455,96 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="34"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="1:7" ht="18">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="31" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="32" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="31" t="s">
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="31" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="41"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="44"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="46"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="45"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="44"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="46"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="45"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="44"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="46"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="45"/>
     </row>
     <row r="9" spans="1:7" ht="52.5" customHeight="1">
-      <c r="A9" s="47"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="49"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="48"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
@@ -1591,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43AD957B-6A27-4937-8EFD-BDCDA705613A}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" activeCellId="1" sqref="F3 F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1613,17 +1619,17 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="35">
+      <c r="B2" s="51"/>
+      <c r="C2" s="34">
         <v>5</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="69" t="s">
         <v>34</v>
       </c>
       <c r="G2" s="10">
@@ -1632,17 +1638,17 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="18">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="37" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="69" t="s">
         <v>35</v>
       </c>
       <c r="G3" s="10">
@@ -1651,233 +1657,227 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="18">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="11"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7" ht="18">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="55"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="54"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="42"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="44"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="46"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="45"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="44"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="46"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="45"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="44"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="46"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="45"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="47"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="49"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="48"/>
     </row>
     <row r="12" spans="1:7" ht="18">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="69" t="s">
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="55"/>
+      <c r="G12" s="54"/>
     </row>
     <row r="13" spans="1:7" ht="16.5">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="52" t="s">
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="43"/>
+      <c r="G13" s="42"/>
     </row>
     <row r="14" spans="1:7" ht="18">
-      <c r="A14" s="18"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="46"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="45"/>
     </row>
     <row r="15" spans="1:7" ht="18">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="46"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="45"/>
     </row>
     <row r="16" spans="1:7" ht="18">
-      <c r="A16" s="18"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="46"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="45"/>
     </row>
     <row r="17" spans="1:7" ht="33">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="49"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="1:7" ht="18">
-      <c r="A18" s="18"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="54" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="55"/>
+      <c r="G18" s="54"/>
     </row>
     <row r="19" spans="1:7" ht="15.75">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="57" t="s">
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="58"/>
+      <c r="G19" s="63"/>
     </row>
     <row r="20" spans="1:7" ht="18">
-      <c r="A20" s="18"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="60"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="65"/>
     </row>
     <row r="21" spans="1:7" ht="18">
-      <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="60"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="65"/>
     </row>
     <row r="22" spans="1:7" ht="18">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="60"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="65"/>
     </row>
     <row r="23" spans="1:7" ht="18">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="60"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="65"/>
     </row>
     <row r="24" spans="1:7" ht="18">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="30" t="str">
+      <c r="B24" s="29" t="str">
         <f>"@impresionescaptis"</f>
         <v>@impresionescaptis</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="62"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:G10"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="F12:G12"/>
     <mergeCell ref="B13:E14"/>
     <mergeCell ref="F13:G17"/>
     <mergeCell ref="B17:E18"/>
@@ -1885,6 +1885,12 @@
     <mergeCell ref="B19:E20"/>
     <mergeCell ref="F19:G24"/>
     <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G10"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="F12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>